<commit_message>
adding link to heroku deployment
</commit_message>
<xml_diff>
--- a/static/input_files/acfrs/CA_Clayton_2022.xlsx
+++ b/static/input_files/acfrs/CA_Clayton_2022.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/input_files/afcrs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/static/input_files/acfrs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B175915-7FF3-0C46-BAF2-D37992959F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B69B25-C94B-7C4C-8067-403B8C12A3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="1080" windowWidth="25200" windowHeight="14360" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31880" yWindow="-7340" windowWidth="25200" windowHeight="14360" tabRatio="834" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement of Net Position" sheetId="1" r:id="rId1"/>
@@ -1721,7 +1721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -2519,7 +2519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -3425,6 +3425,16 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
     <mergeCell ref="E40:F40"/>
     <mergeCell ref="E41:F41"/>
     <mergeCell ref="E35:F35"/>
@@ -3432,16 +3442,6 @@
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3453,12 +3453,12 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="82" style="16" customWidth="1"/>
+    <col min="1" max="1" width="37.33203125" style="16" customWidth="1"/>
     <col min="2" max="2" width="38.83203125" style="16" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" style="16" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="16" customWidth="1"/>
@@ -4508,7 +4508,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="75.33203125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="36" style="16" customWidth="1"/>
     <col min="2" max="2" width="38" style="16" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" style="16" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="16" customWidth="1"/>
@@ -5391,7 +5391,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -5673,8 +5673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -5996,7 +5996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
statement of net position excel
</commit_message>
<xml_diff>
--- a/static/input_files/acfrs/CA_Clayton_2022.xlsx
+++ b/static/input_files/acfrs/CA_Clayton_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/static/input_files/acfrs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E9B1F0-67FB-4F4A-A873-823EC2114A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B042B5-5981-754C-AC3F-9CF88EE8921D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14940" yWindow="-9360" windowWidth="14940" windowHeight="21600" tabRatio="834" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18640" yWindow="-9360" windowWidth="18640" windowHeight="21600" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement of Net Position" sheetId="1" r:id="rId1"/>
@@ -1722,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -3453,8 +3453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>

</xml_diff>